<commit_message>
comparison graphs, 1s analsys
</commit_message>
<xml_diff>
--- a/analysis/compare.xlsx
+++ b/analysis/compare.xlsx
@@ -1,14 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="31540" windowHeight="20080" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="fib" sheetId="1" r:id="rId1"/>
-    <sheet name="down" sheetId="2" r:id="rId2"/>
+    <sheet name="Fib Chart" sheetId="3" r:id="rId1"/>
+    <sheet name="fib" sheetId="1" r:id="rId2"/>
+    <sheet name="Down Chart" sheetId="4" r:id="rId3"/>
+    <sheet name="down" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>thread_count</t>
   </si>
@@ -53,6 +55,9 @@
   </si>
   <si>
     <t>10s</t>
+  </si>
+  <si>
+    <t>1s</t>
   </si>
 </sst>
 </file>
@@ -135,9 +140,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -145,45 +154,107 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="22">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <font>
@@ -231,55 +302,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
@@ -292,13 +314,32 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="133"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="33"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>25th Fibonacci</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -388,7 +429,7 @@
             <c:numRef>
               <c:f>fib!$C$2:$C$19</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>94.33333333333333</c:v>
@@ -530,7 +571,7 @@
             <c:numRef>
               <c:f>fib!$E$2:$E$19</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>99.33333333333333</c:v>
@@ -672,7 +713,7 @@
             <c:numRef>
               <c:f>fib!$H$2:$H$19</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>103.0</c:v>
@@ -737,7 +778,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table1[[#Headers],[10s]]</c:f>
+              <c:f>fib!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -749,7 +790,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Table1[10s]</c:f>
+              <c:f>fib!$K$2:$K$19</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="18"/>
@@ -806,6 +847,85 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>21284.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fib!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>fib!$L$2:$L$19</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>206.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>447.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>785.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1076.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1736.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2279.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3522.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4018.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4760.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6862.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9599.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11370.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14356.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18526.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19508.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20535.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>22152.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -820,21 +940,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2127396504"/>
-        <c:axId val="2130687336"/>
+        <c:axId val="2118371272"/>
+        <c:axId val="2020073288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2127396504"/>
+        <c:axId val="2118371272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130687336"/>
+        <c:crossAx val="2020073288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -842,36 +962,51 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2130687336"/>
+        <c:axId val="2020073288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Request Latency (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127396504"/>
+        <c:crossAx val="2118371272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -882,13 +1017,32 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="133"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="33"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>5MB Download</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -913,7 +1067,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Table2[thread_count]</c:f>
+              <c:f>down!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -978,7 +1132,7 @@
             <c:numRef>
               <c:f>down!$B$2:$B$19</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>82.0</c:v>
@@ -1055,7 +1209,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Table2[thread_count]</c:f>
+              <c:f>down!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -1120,7 +1274,7 @@
             <c:numRef>
               <c:f>down!$D$2:$D$19</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>80.66666666666667</c:v>
@@ -1197,7 +1351,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Table2[thread_count]</c:f>
+              <c:f>down!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -1262,7 +1416,7 @@
             <c:numRef>
               <c:f>down!$G$2:$G$19</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>76.0</c:v>
@@ -1317,6 +1471,164 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>18704.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>down!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>down!$I$2:$I$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>81.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>125.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>132.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>146.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>254.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>312.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>356.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>588.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>813.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>883.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5500.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12268.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14308.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15770.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17868.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>down!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>down!$J$2:$J$19</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>125.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>123.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>138.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>153.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>266.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>315.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>358.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>553.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>751.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>870.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5506.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12565.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14390.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15984.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18459.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1331,21 +1643,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2130335848"/>
-        <c:axId val="2130338888"/>
+        <c:axId val="2075692632"/>
+        <c:axId val="2116398808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2130335848"/>
+        <c:axId val="2075692632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130338888"/>
+        <c:crossAx val="2116398808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1353,64 +1665,92 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2130338888"/>
+        <c:axId val="2116398808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Request</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Latency (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130335848"/>
+        <c:crossAx val="2075692632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:dispUnits>
-          <c:builtInUnit val="thousands"/>
-          <c:dispUnitsLbl>
-            <c:layout/>
-          </c:dispUnitsLbl>
-        </c:dispUnits>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>971550</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8570643" cy="5830117"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1423,29 +1763,21 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8570643" cy="5830117"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1458,62 +1790,65 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K19" totalsRowShown="0">
-  <autoFilter ref="A1:K19"/>
-  <tableColumns count="11">
-    <tableColumn id="1" name="thread_count" dataDxfId="10"/>
-    <tableColumn id="9" name="thread%d" dataDxfId="9" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L19" totalsRowShown="0">
+  <autoFilter ref="A1:L19"/>
+  <tableColumns count="12">
+    <tableColumn id="1" name="thread_count" dataDxfId="21"/>
+    <tableColumn id="9" name="thread%d" dataDxfId="20" dataCellStyle="Percent">
       <calculatedColumnFormula>(A2-A1)/A1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="baseline" dataDxfId="8"/>
-    <tableColumn id="8" name="baseline%d" dataDxfId="7" dataCellStyle="Percent">
+    <tableColumn id="2" name="baseline" dataDxfId="19"/>
+    <tableColumn id="8" name="baseline%d" dataDxfId="18" dataCellStyle="Percent">
       <calculatedColumnFormula>(C2-C1)/C1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="5m" dataDxfId="6"/>
-    <tableColumn id="7" name="5m%d" dataDxfId="5" dataCellStyle="Percent">
+    <tableColumn id="3" name="5m" dataDxfId="17"/>
+    <tableColumn id="7" name="5m%d" dataDxfId="16" dataCellStyle="Percent">
       <calculatedColumnFormula>(E2-E1)/E1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="5m%+" dataDxfId="4" dataCellStyle="Percent">
+    <tableColumn id="5" name="5m%+" dataDxfId="15" dataCellStyle="Percent">
       <calculatedColumnFormula>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="1m" dataDxfId="3"/>
-    <tableColumn id="10" name="1m%d" dataDxfId="2" dataCellStyle="Percent">
+    <tableColumn id="4" name="1m" dataDxfId="14"/>
+    <tableColumn id="10" name="1m%d" dataDxfId="13" dataCellStyle="Percent">
       <calculatedColumnFormula>(H2-H1)/H1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="1m%+" dataDxfId="1" dataCellStyle="Percent">
+    <tableColumn id="6" name="1m%+" dataDxfId="12" dataCellStyle="Percent">
       <calculatedColumnFormula>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="10s" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="11" name="10s" dataDxfId="11" dataCellStyle="Percent"/>
+    <tableColumn id="12" name="1s" dataDxfId="10" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H19" totalsRowShown="0">
-  <autoFilter ref="A1:H19"/>
-  <tableColumns count="8">
-    <tableColumn id="1" name="thread_count" dataDxfId="18"/>
-    <tableColumn id="2" name="baseline" dataDxfId="15"/>
-    <tableColumn id="8" name="baseline%d" dataDxfId="14" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J19" totalsRowShown="0">
+  <autoFilter ref="A1:J19"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="thread_count" dataDxfId="8"/>
+    <tableColumn id="2" name="baseline" dataDxfId="7"/>
+    <tableColumn id="8" name="baseline%d" dataDxfId="6" dataCellStyle="Percent">
       <calculatedColumnFormula>(B2-B1)/B1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="5m" dataDxfId="13"/>
-    <tableColumn id="7" name="5m%d" dataDxfId="11" dataCellStyle="Percent">
+    <tableColumn id="3" name="5m" dataDxfId="5"/>
+    <tableColumn id="7" name="5m%d" dataDxfId="4" dataCellStyle="Percent">
       <calculatedColumnFormula>(D2-D1)/D1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="5m%+" dataDxfId="12" dataCellStyle="Percent">
+    <tableColumn id="4" name="5m%+" dataDxfId="3" dataCellStyle="Percent">
       <calculatedColumnFormula>(Table2[[#This Row],[5m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="1m" dataDxfId="17"/>
-    <tableColumn id="6" name="1m%+" dataDxfId="16" dataCellStyle="Percent">
+    <tableColumn id="5" name="1m" dataDxfId="1"/>
+    <tableColumn id="6" name="1m%+" dataDxfId="2" dataCellStyle="Percent">
       <calculatedColumnFormula>(Table2[[#This Row],[1m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="9" name="10s" dataDxfId="9" dataCellStyle="Percent"/>
+    <tableColumn id="10" name="1s" dataDxfId="0" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1841,22 +2176,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AB25" sqref="AB25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1890,21 +2229,24 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>2</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="4">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="6">
         <v>94.333333333333329</v>
       </c>
       <c r="D2" s="5">
         <v>0</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="6">
         <v>99.333333333333329</v>
       </c>
       <c r="F2" s="5">
@@ -1914,7 +2256,7 @@
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>5.3003533568904596E-2</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="6">
         <v>103</v>
       </c>
       <c r="I2" s="5">
@@ -1924,26 +2266,29 @@
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>9.1872791519434685E-2</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="5">
         <v>104</v>
       </c>
+      <c r="L2" s="5">
+        <v>97.5</v>
+      </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>4</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="4">
         <f t="shared" ref="B3:B19" si="0">(A3-A2)/A2</f>
         <v>1</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="6">
         <v>224</v>
       </c>
       <c r="D3" s="5">
         <f t="shared" ref="D3:D19" si="1">(C3-C2)/C2</f>
         <v>1.374558303886926</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="6">
         <v>227.66666666666666</v>
       </c>
       <c r="F3" s="5">
@@ -1954,37 +2299,40 @@
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>1.6369047619047578E-2</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="6">
         <v>243.33333333333334</v>
       </c>
       <c r="I3" s="5">
-        <f t="shared" ref="I2:I19" si="3">(H3-H2)/H2</f>
+        <f t="shared" ref="I3:I19" si="3">(H3-H2)/H2</f>
         <v>1.3624595469255665</v>
       </c>
       <c r="J3" s="5">
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>8.630952380952385E-2</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="5">
         <v>200</v>
       </c>
+      <c r="L3" s="5">
+        <v>206</v>
+      </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>8</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="6">
         <v>449.66666666666669</v>
       </c>
       <c r="D4" s="5">
         <f t="shared" si="1"/>
         <v>1.0074404761904763</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="6">
         <v>454</v>
       </c>
       <c r="F4" s="5">
@@ -1995,7 +2343,7 @@
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>9.6367679762786821E-3</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="6">
         <v>594</v>
       </c>
       <c r="I4" s="5">
@@ -2006,26 +2354,29 @@
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.32097850259451438</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="5">
         <v>436</v>
       </c>
+      <c r="L4" s="5">
+        <v>447</v>
+      </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>12</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="4">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="6">
         <v>726.66666666666663</v>
       </c>
       <c r="D5" s="5">
         <f t="shared" si="1"/>
         <v>0.61601186063750912</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="6">
         <v>744.33333333333337</v>
       </c>
       <c r="F5" s="5">
@@ -2036,7 +2387,7 @@
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>2.4311926605504693E-2</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="6">
         <v>988.66666666666663</v>
       </c>
       <c r="I5" s="5">
@@ -2047,26 +2398,29 @@
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.36055045871559632</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="5">
         <v>717</v>
       </c>
+      <c r="L5" s="5">
+        <v>785.5</v>
+      </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>16</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="4">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="6">
         <v>1012.6666666666666</v>
       </c>
       <c r="D6" s="5">
         <f t="shared" si="1"/>
         <v>0.39357798165137614</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="6">
         <v>1043</v>
       </c>
       <c r="F6" s="5">
@@ -2077,7 +2431,7 @@
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>2.9953917050691281E-2</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="6">
         <v>1337.6666666666667</v>
       </c>
       <c r="I6" s="5">
@@ -2088,26 +2442,29 @@
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.32093482554312058</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="5">
         <v>1042</v>
       </c>
+      <c r="L6" s="5">
+        <v>1076.5</v>
+      </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>24</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="4">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="6">
         <v>1586.3333333333333</v>
       </c>
       <c r="D7" s="5">
         <f t="shared" si="1"/>
         <v>0.56649111257406182</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="6">
         <v>1650.6666666666667</v>
       </c>
       <c r="F7" s="5">
@@ -2118,7 +2475,7 @@
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>4.0554738390418253E-2</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="6">
         <v>2096.3333333333335</v>
       </c>
       <c r="I7" s="5">
@@ -2129,26 +2486,29 @@
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.32149611262870365</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="5">
         <v>1640</v>
       </c>
+      <c r="L7" s="5">
+        <v>1736</v>
+      </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <v>32</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="4">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="6">
         <v>2081.6666666666665</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="1"/>
         <v>0.3122504727884009</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="6">
         <v>2314.3333333333335</v>
       </c>
       <c r="F8" s="5">
@@ -2159,7 +2519,7 @@
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.1117694155324261</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="6">
         <v>2794.6666666666665</v>
       </c>
       <c r="I8" s="5">
@@ -2170,26 +2530,29 @@
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.34251401120896718</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="5">
         <v>2221</v>
       </c>
+      <c r="L8" s="5">
+        <v>2279</v>
+      </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <v>48</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="4">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="6">
         <v>3241</v>
       </c>
       <c r="D9" s="5">
         <f t="shared" si="1"/>
         <v>0.55692554043234599</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="6">
         <v>3472.3333333333335</v>
       </c>
       <c r="F9" s="5">
@@ -2200,7 +2563,7 @@
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>7.1377146971099495E-2</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="6">
         <v>4166.333333333333</v>
       </c>
       <c r="I9" s="5">
@@ -2211,26 +2574,29 @@
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.2855085878843977</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="5">
         <v>3541</v>
       </c>
+      <c r="L9" s="5">
+        <v>3522.5</v>
+      </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <v>56</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="6">
         <v>3802</v>
       </c>
       <c r="D10" s="5">
         <f t="shared" si="1"/>
         <v>0.17309472385066338</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="6">
         <v>3942.6666666666665</v>
       </c>
       <c r="F10" s="5">
@@ -2241,7 +2607,7 @@
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>3.6998071190601396E-2</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="6">
         <v>4331.333333333333</v>
       </c>
       <c r="I10" s="5">
@@ -2252,26 +2618,29 @@
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.13922496931439585</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="5">
         <v>3963</v>
       </c>
+      <c r="L10" s="5">
+        <v>4018</v>
+      </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>64</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <f t="shared" si="0"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="6">
         <v>4068</v>
       </c>
       <c r="D11" s="5">
         <f t="shared" si="1"/>
         <v>6.996317727511836E-2</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="6">
         <v>4722</v>
       </c>
       <c r="F11" s="5">
@@ -2282,7 +2651,7 @@
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.16076696165191739</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="6">
         <v>5431</v>
       </c>
       <c r="I11" s="5">
@@ -2293,26 +2662,29 @@
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.33505408062930186</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="5">
         <v>4608</v>
       </c>
+      <c r="L11" s="5">
+        <v>4760</v>
+      </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12">
       <c r="A12" s="1">
         <v>96</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="4">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="6">
         <v>6320.333333333333</v>
       </c>
       <c r="D12" s="5">
         <f t="shared" si="1"/>
         <v>0.5536709275647328</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="6">
         <v>6506</v>
       </c>
       <c r="F12" s="5">
@@ -2323,7 +2695,7 @@
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>2.9376087759084485E-2</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="6">
         <v>8174</v>
       </c>
       <c r="I12" s="5">
@@ -2334,26 +2706,29 @@
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.29328621908127217</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="5">
         <v>7095</v>
       </c>
+      <c r="L12" s="5">
+        <v>6862.5</v>
+      </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:12">
       <c r="A13" s="1">
         <v>128</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="4">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="6">
         <v>8017.333333333333</v>
       </c>
       <c r="D13" s="5">
         <f t="shared" si="1"/>
         <v>0.26849849691471972</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="6">
         <v>9072.3333333333339</v>
       </c>
       <c r="F13" s="5">
@@ -2364,7 +2739,7 @@
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.13158988857475482</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="6">
         <v>10364.333333333334</v>
       </c>
       <c r="I13" s="5">
@@ -2375,26 +2750,29 @@
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.29274072842175297</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="5">
         <v>8944</v>
       </c>
+      <c r="L13" s="5">
+        <v>9599.5</v>
+      </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:12">
       <c r="A14" s="1">
         <v>256</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="6">
         <v>9777.3333333333339</v>
       </c>
       <c r="D14" s="5">
         <f t="shared" si="1"/>
         <v>0.21952436387826388</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="6">
         <v>10369.666666666666</v>
       </c>
       <c r="F14" s="5">
@@ -2405,7 +2783,7 @@
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>6.0582299195417848E-2</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="6">
         <v>11890</v>
       </c>
       <c r="I14" s="5">
@@ -2416,26 +2794,29 @@
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.21607800354561563</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="5">
         <v>11116</v>
       </c>
+      <c r="L14" s="5">
+        <v>11370</v>
+      </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:12">
       <c r="A15" s="1">
         <v>512</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="6">
         <v>12696.666666666666</v>
       </c>
       <c r="D15" s="5">
         <f t="shared" si="1"/>
         <v>0.29858175371607787</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="6">
         <v>13770.333333333334</v>
       </c>
       <c r="F15" s="5">
@@ -2446,7 +2827,7 @@
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>8.4562877395642E-2</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="6">
         <v>15466.333333333334</v>
       </c>
       <c r="I15" s="5">
@@ -2457,26 +2838,29 @@
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.21814124442110802</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="5">
         <v>13754</v>
       </c>
+      <c r="L15" s="5">
+        <v>14356.5</v>
+      </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:12">
       <c r="A16" s="1">
         <v>1024</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="6">
         <v>16797</v>
       </c>
       <c r="D16" s="5">
         <f t="shared" si="1"/>
         <v>0.32294565502756634</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="6">
         <v>17894.666666666668</v>
       </c>
       <c r="F16" s="5">
@@ -2487,7 +2871,7 @@
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>6.5348971046417084E-2</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="6">
         <v>19193.666666666668</v>
       </c>
       <c r="I16" s="5">
@@ -2498,26 +2882,29 @@
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.14268420948185198</v>
       </c>
-      <c r="K16" s="7">
+      <c r="K16" s="5">
         <v>17954</v>
       </c>
+      <c r="L16" s="5">
+        <v>18526.5</v>
+      </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:12">
       <c r="A17" s="1">
         <v>1280</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="4">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="6">
         <v>17989</v>
       </c>
       <c r="D17" s="5">
         <f t="shared" si="1"/>
         <v>7.0965053283324406E-2</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="6">
         <v>19289.666666666668</v>
       </c>
       <c r="F17" s="5">
@@ -2528,7 +2915,7 @@
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>7.2303444697685695E-2</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="6">
         <v>21436</v>
       </c>
       <c r="I17" s="5">
@@ -2539,26 +2926,29 @@
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.19161709933848464</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="5">
         <v>18906</v>
       </c>
+      <c r="L17" s="5">
+        <v>19508</v>
+      </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:12">
       <c r="A18" s="1">
         <v>1536</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="4">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="6">
         <v>19119</v>
       </c>
       <c r="D18" s="5">
         <f t="shared" si="1"/>
         <v>6.281616543443215E-2</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="6">
         <v>19812.333333333332</v>
       </c>
       <c r="F18" s="5">
@@ -2569,7 +2959,7 @@
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>3.6264100284184954E-2</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="6">
         <v>21494.666666666668</v>
       </c>
       <c r="I18" s="5">
@@ -2580,26 +2970,29 @@
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.12425684746412824</v>
       </c>
-      <c r="K18" s="7">
+      <c r="K18" s="5">
         <v>19894</v>
       </c>
+      <c r="L18" s="5">
+        <v>20535</v>
+      </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:12">
       <c r="A19" s="2">
         <v>2048</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="4">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="6">
         <v>20388</v>
       </c>
       <c r="D19" s="5">
         <f t="shared" si="1"/>
         <v>6.6373764318217482E-2</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="6">
         <v>21465.333333333332</v>
       </c>
       <c r="F19" s="5">
@@ -2610,7 +3003,7 @@
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>5.2841540775619589E-2</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="6">
         <v>22838.333333333332</v>
       </c>
       <c r="I19" s="5">
@@ -2621,16 +3014,18 @@
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.12018507618860762</v>
       </c>
-      <c r="K19" s="7">
+      <c r="K19" s="5">
         <v>21284</v>
+      </c>
+      <c r="L19" s="5">
+        <v>22152</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -2642,22 +3037,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2682,551 +3080,664 @@
       <c r="H1" t="s">
         <v>4</v>
       </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>2</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="6">
         <v>82</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="5">
         <v>0</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="6">
         <v>80.666666666666671</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="5">
         <v>0</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="5">
         <f>(Table2[[#This Row],[5m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>-1.6260162601625959E-2</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="6">
         <v>76</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <f>(Table2[[#This Row],[1m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>-7.3170731707317069E-2</v>
       </c>
+      <c r="I2" s="7">
+        <v>80</v>
+      </c>
+      <c r="J2" s="5">
+        <v>68</v>
+      </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>4</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="6">
         <v>80</v>
       </c>
-      <c r="C3" s="4">
-        <f t="shared" ref="C2:C19" si="0">(B3-B2)/B2</f>
+      <c r="C3" s="5">
+        <f t="shared" ref="C3:C19" si="0">(B3-B2)/B2</f>
         <v>-2.4390243902439025E-2</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="6">
         <v>78.666666666666671</v>
       </c>
-      <c r="E3" s="4">
-        <f t="shared" ref="E2:E19" si="1">(D3-D2)/D2</f>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E19" si="1">(D3-D2)/D2</f>
         <v>-2.4793388429752063E-2</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="5">
         <f>(Table2[[#This Row],[5m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>-1.6666666666666607E-2</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="6">
         <v>76</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <f>(Table2[[#This Row],[1m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>-0.05</v>
       </c>
+      <c r="I3" s="7">
+        <v>81</v>
+      </c>
+      <c r="J3" s="5">
+        <v>78</v>
+      </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>8</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="6">
         <v>130.66666666666666</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="5">
         <f t="shared" si="0"/>
         <v>0.63333333333333319</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="6">
         <v>125.33333333333333</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="5">
         <f t="shared" si="1"/>
         <v>0.59322033898305071</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="5">
         <f>(Table2[[#This Row],[5m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>-4.0816326530612214E-2</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="6">
         <v>106.33333333333333</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <f>(Table2[[#This Row],[1m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>-0.18622448979591835</v>
       </c>
+      <c r="I4" s="7">
+        <v>128</v>
+      </c>
+      <c r="J4" s="5">
+        <v>125</v>
+      </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>12</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="6">
         <v>134.33333333333334</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="5">
         <f t="shared" si="0"/>
         <v>2.8061224489796064E-2</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="6">
         <v>123.33333333333333</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="5">
         <f t="shared" si="1"/>
         <v>-1.5957446808510641E-2</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="5">
         <f>(Table2[[#This Row],[5m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>-8.1885856079404573E-2</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="6">
         <v>102.66666666666667</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <f>(Table2[[#This Row],[1m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>-0.23573200992555834</v>
       </c>
+      <c r="I5" s="7">
+        <v>125</v>
+      </c>
+      <c r="J5" s="5">
+        <v>123.5</v>
+      </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>16</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="6">
         <v>132.33333333333334</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="5">
         <f t="shared" si="0"/>
         <v>-1.4888337468982629E-2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="6">
         <v>128</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="5">
         <f t="shared" si="1"/>
         <v>3.7837837837837875E-2</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="5">
         <f>(Table2[[#This Row],[5m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>-3.2745591939546667E-2</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="6">
         <v>109.33333333333333</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <f>(Table2[[#This Row],[1m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>-0.17380352644836281</v>
       </c>
+      <c r="I6" s="7">
+        <v>128</v>
+      </c>
+      <c r="J6" s="5">
+        <v>125</v>
+      </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>24</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="6">
         <v>144</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="5">
         <f t="shared" si="0"/>
         <v>8.8161209068009991E-2</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="6">
         <v>138.33333333333334</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="5">
         <f t="shared" si="1"/>
         <v>8.0729166666666741E-2</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="5">
         <f>(Table2[[#This Row],[5m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>-3.9351851851851784E-2</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="6">
         <v>118</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <f>(Table2[[#This Row],[1m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>-0.18055555555555555</v>
       </c>
+      <c r="I7" s="7">
+        <v>132</v>
+      </c>
+      <c r="J7" s="5">
+        <v>138</v>
+      </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>32</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="6">
         <v>159.66666666666666</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="5">
         <f t="shared" si="0"/>
         <v>0.10879629629629622</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="6">
         <v>144</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="5">
         <f t="shared" si="1"/>
         <v>4.0963855421686679E-2</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="5">
         <f>(Table2[[#This Row],[5m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>-9.8121085594989513E-2</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="6">
         <v>132.33333333333334</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <f>(Table2[[#This Row],[1m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>-0.17118997912317316</v>
       </c>
+      <c r="I8" s="7">
+        <v>146</v>
+      </c>
+      <c r="J8" s="5">
+        <v>153</v>
+      </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>48</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="6">
         <v>268</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="5">
         <f t="shared" si="0"/>
         <v>0.67849686847599178</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="6">
         <v>268</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="5">
         <f t="shared" si="1"/>
         <v>0.86111111111111116</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="5">
         <f>(Table2[[#This Row],[5m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>0</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="6">
         <v>261.33333333333331</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <f>(Table2[[#This Row],[1m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>-2.4875621890547334E-2</v>
       </c>
+      <c r="I9" s="7">
+        <v>254</v>
+      </c>
+      <c r="J9" s="5">
+        <v>266.5</v>
+      </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>56</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="6">
         <v>315</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="5">
         <f t="shared" si="0"/>
         <v>0.17537313432835822</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="6">
         <v>314</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="5">
         <f t="shared" si="1"/>
         <v>0.17164179104477612</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="5">
         <f>(Table2[[#This Row],[5m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>-3.1746031746031746E-3</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="6">
         <v>364</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <f>(Table2[[#This Row],[1m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>0.15555555555555556</v>
       </c>
+      <c r="I10" s="7">
+        <v>312</v>
+      </c>
+      <c r="J10" s="5">
+        <v>315</v>
+      </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>64</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="6">
         <v>361.66666666666669</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="5">
         <f t="shared" si="0"/>
         <v>0.1481481481481482</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="6">
         <v>368</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="5">
         <f t="shared" si="1"/>
         <v>0.17197452229299362</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="5">
         <f>(Table2[[#This Row],[5m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>1.7511520737327136E-2</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="6">
         <v>365.33333333333331</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <f>(Table2[[#This Row],[1m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>1.0138248847926162E-2</v>
       </c>
+      <c r="I11" s="7">
+        <v>356</v>
+      </c>
+      <c r="J11" s="5">
+        <v>358.5</v>
+      </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>96</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="6">
         <v>598</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="5">
         <f t="shared" si="0"/>
         <v>0.65345622119815661</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="6">
         <v>584</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="5">
         <f t="shared" si="1"/>
         <v>0.58695652173913049</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="5">
         <f>(Table2[[#This Row],[5m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>-2.3411371237458192E-2</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="6">
         <v>575.33333333333337</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <f>(Table2[[#This Row],[1m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>-3.7904124860646538E-2</v>
       </c>
+      <c r="I12" s="7">
+        <v>588</v>
+      </c>
+      <c r="J12" s="5">
+        <v>553.5</v>
+      </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>128</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="6">
         <v>858.66666666666663</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="5">
         <f t="shared" si="0"/>
         <v>0.43589743589743585</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="6">
         <v>857</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="5">
         <f t="shared" si="1"/>
         <v>0.46746575342465752</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="5">
         <f>(Table2[[#This Row],[5m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>-1.9409937888198317E-3</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="6">
         <v>801.33333333333337</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="3">
         <f>(Table2[[#This Row],[1m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>-6.6770186335403645E-2</v>
       </c>
+      <c r="I13" s="7">
+        <v>813</v>
+      </c>
+      <c r="J13" s="5">
+        <v>751</v>
+      </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>256</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="6">
         <v>1037</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="5">
         <f t="shared" si="0"/>
         <v>0.20768633540372677</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="6">
         <v>991</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="5">
         <f t="shared" si="1"/>
         <v>0.15635939323220538</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="5">
         <f>(Table2[[#This Row],[5m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>-4.4358727097396335E-2</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="6">
         <v>1072.6666666666667</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="3">
         <f>(Table2[[#This Row],[1m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>3.4394085503053756E-2</v>
       </c>
+      <c r="I14" s="7">
+        <v>883</v>
+      </c>
+      <c r="J14" s="5">
+        <v>870</v>
+      </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>512</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="6">
         <v>5583.666666666667</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="5">
         <f t="shared" si="0"/>
         <v>4.3844423015107683</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="6">
         <v>5765.666666666667</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="5">
         <f t="shared" si="1"/>
         <v>4.8180289270097552</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="5">
         <f>(Table2[[#This Row],[5m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>3.2595068951107392E-2</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="6">
         <v>6016.333333333333</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <f>(Table2[[#This Row],[1m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>7.748791116948231E-2</v>
       </c>
+      <c r="I15" s="7">
+        <v>5500</v>
+      </c>
+      <c r="J15" s="5">
+        <v>5506.5</v>
+      </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>1024</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="6">
         <v>11548</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="5">
         <f t="shared" si="0"/>
         <v>1.0681750343263088</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="6">
         <v>12266.666666666666</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="5">
         <f t="shared" si="1"/>
         <v>1.1275365670347457</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="5">
         <f>(Table2[[#This Row],[5m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>6.2232998499018539E-2</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="6">
         <v>12725.666666666666</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="3">
         <f>(Table2[[#This Row],[1m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>0.10198014086133236</v>
       </c>
+      <c r="I16" s="7">
+        <v>12268</v>
+      </c>
+      <c r="J16" s="5">
+        <v>12565.5</v>
+      </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>1280</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="6">
         <v>13511.666666666666</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="5">
         <f t="shared" si="0"/>
         <v>0.17004387484124231</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="6">
         <v>14421</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="5">
         <f t="shared" si="1"/>
         <v>0.17562500000000006</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="5">
         <f>(Table2[[#This Row],[5m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>6.7299864314789737E-2</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="6">
         <v>15276</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="3">
         <f>(Table2[[#This Row],[1m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>0.13057851239669427</v>
       </c>
+      <c r="I17" s="7">
+        <v>14308</v>
+      </c>
+      <c r="J17" s="5">
+        <v>14390</v>
+      </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>1536</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="6">
         <v>14754</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="5">
         <f t="shared" si="0"/>
         <v>9.1945232515110442E-2</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="6">
         <v>15327.333333333334</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="5">
         <f t="shared" si="1"/>
         <v>6.2848161246330622E-2</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="5">
         <f>(Table2[[#This Row],[5m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>3.8859518322714788E-2</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="6">
         <v>16505.666666666668</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="3">
         <f>(Table2[[#This Row],[1m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>0.11872486557317798</v>
       </c>
+      <c r="I18" s="7">
+        <v>15770</v>
+      </c>
+      <c r="J18" s="5">
+        <v>15984</v>
+      </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:10">
       <c r="A19" s="2">
         <v>2048</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="6">
         <v>17103.333333333332</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="5">
         <f t="shared" si="0"/>
         <v>0.15923365415028684</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="6">
         <v>17981.333333333332</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="5">
         <f t="shared" si="1"/>
         <v>0.17315471271367044</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="5">
         <f>(Table2[[#This Row],[5m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>5.1335022412785036E-2</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="6">
         <v>18704</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="3">
         <f>(Table2[[#This Row],[1m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</f>
         <v>9.3587994542974159E-2</v>
+      </c>
+      <c r="I19" s="7">
+        <v>17868</v>
+      </c>
+      <c r="J19" s="5">
+        <v>18459</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
network analysis and graphs
</commit_message>
<xml_diff>
--- a/analysis/compare.xlsx
+++ b/analysis/compare.xlsx
@@ -175,10 +175,13 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -222,9 +225,6 @@
         </top>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -314,33 +314,14 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="133"/>
+      <c14:style val="134"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="33"/>
+      <c:style val="34"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>25th Fibonacci</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -940,11 +921,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2118371272"/>
-        <c:axId val="2020073288"/>
+        <c:axId val="2115819608"/>
+        <c:axId val="2115822728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2118371272"/>
+        <c:axId val="2115819608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -954,7 +935,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2020073288"/>
+        <c:crossAx val="2115822728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -962,7 +943,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2020073288"/>
+        <c:axId val="2115822728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -992,7 +973,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118371272"/>
+        <c:crossAx val="2115819608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1017,33 +998,14 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="133"/>
+      <c14:style val="134"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="33"/>
+      <c:style val="34"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>5MB Download</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1643,11 +1605,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2075692632"/>
-        <c:axId val="2116398808"/>
+        <c:axId val="2115965720"/>
+        <c:axId val="2115968840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2075692632"/>
+        <c:axId val="2115965720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1657,7 +1619,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116398808"/>
+        <c:crossAx val="2115968840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1665,7 +1627,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2116398808"/>
+        <c:axId val="2115968840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1683,13 +1645,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Request</a:t>
+                  <a:t>Request Latency (ms)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Latency (ms)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1700,7 +1657,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2075692632"/>
+        <c:crossAx val="2115965720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1725,6 +1682,7 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
 </chartsheet>
 </file>
@@ -1736,6 +1694,7 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
 </chartsheet>
 </file>
@@ -1744,7 +1703,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8570643" cy="5830117"/>
+    <xdr:ext cx="8572500" cy="5829300"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1771,7 +1730,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8570643" cy="5830117"/>
+    <xdr:ext cx="8572500" cy="5829300"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1831,23 +1790,23 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J19" totalsRowShown="0">
   <autoFilter ref="A1:J19"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="thread_count" dataDxfId="8"/>
-    <tableColumn id="2" name="baseline" dataDxfId="7"/>
-    <tableColumn id="8" name="baseline%d" dataDxfId="6" dataCellStyle="Percent">
+    <tableColumn id="1" name="thread_count" dataDxfId="9"/>
+    <tableColumn id="2" name="baseline" dataDxfId="8"/>
+    <tableColumn id="8" name="baseline%d" dataDxfId="7" dataCellStyle="Percent">
       <calculatedColumnFormula>(B2-B1)/B1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="5m" dataDxfId="5"/>
-    <tableColumn id="7" name="5m%d" dataDxfId="4" dataCellStyle="Percent">
+    <tableColumn id="3" name="5m" dataDxfId="6"/>
+    <tableColumn id="7" name="5m%d" dataDxfId="5" dataCellStyle="Percent">
       <calculatedColumnFormula>(D2-D1)/D1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="5m%+" dataDxfId="3" dataCellStyle="Percent">
+    <tableColumn id="4" name="5m%+" dataDxfId="4" dataCellStyle="Percent">
       <calculatedColumnFormula>(Table2[[#This Row],[5m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="1m" dataDxfId="1"/>
+    <tableColumn id="5" name="1m" dataDxfId="3"/>
     <tableColumn id="6" name="1m%+" dataDxfId="2" dataCellStyle="Percent">
       <calculatedColumnFormula>(Table2[[#This Row],[1m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="10s" dataDxfId="9" dataCellStyle="Percent"/>
+    <tableColumn id="9" name="10s" dataDxfId="1" dataCellStyle="Percent"/>
     <tableColumn id="10" name="1s" dataDxfId="0" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>

</xml_diff>

<commit_message>
first draft of analysis write up
</commit_message>
<xml_diff>
--- a/analysis/compare.xlsx
+++ b/analysis/compare.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>thread_count</t>
   </si>
@@ -59,6 +59,18 @@
   <si>
     <t>1s</t>
   </si>
+  <si>
+    <t>10s%d</t>
+  </si>
+  <si>
+    <t>1s%d</t>
+  </si>
+  <si>
+    <t>10s%+</t>
+  </si>
+  <si>
+    <t>1s%+</t>
+  </si>
 </sst>
 </file>
 
@@ -67,7 +79,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -94,6 +106,14 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -150,7 +170,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -159,6 +179,12 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -170,7 +196,72 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -225,33 +316,6 @@
         </top>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -838,7 +902,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>fib!$L$1</c:f>
+              <c:f>fib!$N$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -850,7 +914,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>fib!$L$2:$L$19</c:f>
+              <c:f>fib!$N$2:$N$19</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="18"/>
@@ -921,11 +985,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2115819608"/>
-        <c:axId val="2115822728"/>
+        <c:axId val="2108547096"/>
+        <c:axId val="2081816328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2115819608"/>
+        <c:axId val="2108547096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -935,7 +999,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115822728"/>
+        <c:crossAx val="2081816328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -943,7 +1007,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115822728"/>
+        <c:axId val="2081816328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -973,7 +1037,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115819608"/>
+        <c:crossAx val="2108547096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1605,11 +1669,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2115965720"/>
-        <c:axId val="2115968840"/>
+        <c:axId val="2106910440"/>
+        <c:axId val="2106913560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2115965720"/>
+        <c:axId val="2106910440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1619,7 +1683,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115968840"/>
+        <c:crossAx val="2106913560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1627,7 +1691,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115968840"/>
+        <c:axId val="2106913560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1657,7 +1721,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115965720"/>
+        <c:crossAx val="2106910440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1679,7 +1743,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1691,7 +1755,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="150" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1754,33 +1818,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L19" totalsRowShown="0">
-  <autoFilter ref="A1:L19"/>
-  <tableColumns count="12">
-    <tableColumn id="1" name="thread_count" dataDxfId="21"/>
-    <tableColumn id="9" name="thread%d" dataDxfId="20" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:P19" totalsRowShown="0">
+  <autoFilter ref="A1:P19"/>
+  <tableColumns count="16">
+    <tableColumn id="1" name="thread_count" dataDxfId="24"/>
+    <tableColumn id="9" name="thread%d" dataDxfId="23" dataCellStyle="Percent">
       <calculatedColumnFormula>(A2-A1)/A1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="baseline" dataDxfId="19"/>
-    <tableColumn id="8" name="baseline%d" dataDxfId="18" dataCellStyle="Percent">
+    <tableColumn id="2" name="baseline" dataDxfId="10"/>
+    <tableColumn id="8" name="baseline%d" dataDxfId="8" dataCellStyle="Percent">
       <calculatedColumnFormula>(C2-C1)/C1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="5m" dataDxfId="17"/>
-    <tableColumn id="7" name="5m%d" dataDxfId="16" dataCellStyle="Percent">
+    <tableColumn id="3" name="5m" dataDxfId="9"/>
+    <tableColumn id="7" name="5m%d" dataDxfId="7" dataCellStyle="Percent">
       <calculatedColumnFormula>(E2-E1)/E1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="5m%+" dataDxfId="15" dataCellStyle="Percent">
+    <tableColumn id="5" name="5m%+" dataDxfId="4" dataCellStyle="Percent">
       <calculatedColumnFormula>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="1m" dataDxfId="14"/>
-    <tableColumn id="10" name="1m%d" dataDxfId="13" dataCellStyle="Percent">
+    <tableColumn id="4" name="1m" dataDxfId="6"/>
+    <tableColumn id="10" name="1m%d" dataDxfId="11" dataCellStyle="Percent">
       <calculatedColumnFormula>(H2-H1)/H1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="1m%+" dataDxfId="12" dataCellStyle="Percent">
+    <tableColumn id="6" name="1m%+" dataDxfId="5" dataCellStyle="Percent">
       <calculatedColumnFormula>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="10s" dataDxfId="11" dataCellStyle="Percent"/>
-    <tableColumn id="12" name="1s" dataDxfId="10" dataCellStyle="Percent"/>
+    <tableColumn id="11" name="10s" dataDxfId="22" dataCellStyle="Percent"/>
+    <tableColumn id="13" name="10s%d" dataDxfId="2" dataCellStyle="Percent"/>
+    <tableColumn id="15" name="10s%+" dataDxfId="0" dataCellStyle="Percent">
+      <calculatedColumnFormula>(Table1[[#This Row],[10s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" name="1s" dataDxfId="1" dataCellStyle="Percent"/>
+    <tableColumn id="14" name="1s%d" dataCellStyle="Percent"/>
+    <tableColumn id="16" name="1s%+" dataDxfId="3" dataCellStyle="Percent">
+      <calculatedColumnFormula>(Table1[[#This Row],[1s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1790,24 +1862,24 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J19" totalsRowShown="0">
   <autoFilter ref="A1:J19"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="thread_count" dataDxfId="9"/>
-    <tableColumn id="2" name="baseline" dataDxfId="8"/>
-    <tableColumn id="8" name="baseline%d" dataDxfId="7" dataCellStyle="Percent">
+    <tableColumn id="1" name="thread_count" dataDxfId="21"/>
+    <tableColumn id="2" name="baseline" dataDxfId="20"/>
+    <tableColumn id="8" name="baseline%d" dataDxfId="19" dataCellStyle="Percent">
       <calculatedColumnFormula>(B2-B1)/B1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="5m" dataDxfId="6"/>
-    <tableColumn id="7" name="5m%d" dataDxfId="5" dataCellStyle="Percent">
+    <tableColumn id="3" name="5m" dataDxfId="18"/>
+    <tableColumn id="7" name="5m%d" dataDxfId="17" dataCellStyle="Percent">
       <calculatedColumnFormula>(D2-D1)/D1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="5m%+" dataDxfId="4" dataCellStyle="Percent">
+    <tableColumn id="4" name="5m%+" dataDxfId="16" dataCellStyle="Percent">
       <calculatedColumnFormula>(Table2[[#This Row],[5m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="1m" dataDxfId="3"/>
-    <tableColumn id="6" name="1m%+" dataDxfId="2" dataCellStyle="Percent">
+    <tableColumn id="5" name="1m" dataDxfId="15"/>
+    <tableColumn id="6" name="1m%+" dataDxfId="14" dataCellStyle="Percent">
       <calculatedColumnFormula>(Table2[[#This Row],[1m]]-Table2[[#This Row],[baseline]])/Table2[[#This Row],[baseline]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="10s" dataDxfId="1" dataCellStyle="Percent"/>
-    <tableColumn id="10" name="1s" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="9" name="10s" dataDxfId="13" dataCellStyle="Percent"/>
+    <tableColumn id="10" name="1s" dataDxfId="12" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2135,33 +2207,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AB25" sqref="AB25"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
     <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="9" customWidth="1"/>
     <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9" hidden="1" customWidth="1"/>
+    <col min="9" max="10" width="9" customWidth="1"/>
     <col min="11" max="11" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11.5" customWidth="1"/>
+    <col min="14" max="14" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
@@ -2189,50 +2262,76 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
         <v>11</v>
       </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:16">
       <c r="A2" s="1">
         <v>2</v>
       </c>
       <c r="B2" s="4">
         <v>0</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="12">
         <v>94.333333333333329</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="10">
         <v>0</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="12">
         <v>99.333333333333329</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="10">
         <v>0</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="8">
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>5.3003533568904596E-2</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="12">
         <v>103</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="10">
         <v>0</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="8">
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>9.1872791519434685E-2</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="13">
         <v>104</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="8">
+        <v>0</v>
+      </c>
+      <c r="M2" s="9">
+        <f>(Table1[[#This Row],[10s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>0.10247349823321561</v>
+      </c>
+      <c r="N2" s="13">
         <v>97.5</v>
       </c>
+      <c r="O2" s="8">
+        <v>0</v>
+      </c>
+      <c r="P2" s="9">
+        <f>(Table1[[#This Row],[1s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>3.3568904593639627E-2</v>
+      </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:16">
       <c r="A3" s="1">
         <v>4</v>
       </c>
@@ -2240,43 +2339,59 @@
         <f t="shared" ref="B3:B19" si="0">(A3-A2)/A2</f>
         <v>1</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="12">
         <v>224</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="10">
         <f t="shared" ref="D3:D19" si="1">(C3-C2)/C2</f>
         <v>1.374558303886926</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="12">
         <v>227.66666666666666</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="10">
         <f t="shared" ref="F3:F19" si="2">(E3-E2)/E2</f>
         <v>1.2919463087248322</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="8">
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>1.6369047619047578E-2</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="12">
         <v>243.33333333333334</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="10">
         <f t="shared" ref="I3:I19" si="3">(H3-H2)/H2</f>
         <v>1.3624595469255665</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="8">
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>8.630952380952385E-2</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="13">
         <v>200</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="8">
+        <f>(K3-K2)/K2</f>
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="M3" s="9">
+        <f>(Table1[[#This Row],[10s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>-0.10714285714285714</v>
+      </c>
+      <c r="N3" s="13">
         <v>206</v>
       </c>
+      <c r="O3" s="8">
+        <f>(N3-N2)/N2</f>
+        <v>1.1128205128205129</v>
+      </c>
+      <c r="P3" s="9">
+        <f>(Table1[[#This Row],[1s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>-8.0357142857142863E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:16">
       <c r="A4" s="1">
         <v>8</v>
       </c>
@@ -2284,43 +2399,59 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="12">
         <v>449.66666666666669</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="10">
         <f t="shared" si="1"/>
         <v>1.0074404761904763</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="12">
         <v>454</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="10">
         <f t="shared" si="2"/>
         <v>0.99414348462664726</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="8">
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>9.6367679762786821E-3</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="12">
         <v>594</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="10">
         <f t="shared" si="3"/>
         <v>1.4410958904109588</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="8">
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.32097850259451438</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="13">
         <v>436</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="8">
+        <f t="shared" ref="L4:L19" si="4">(K4-K3)/K3</f>
+        <v>1.18</v>
+      </c>
+      <c r="M4" s="9">
+        <f>(Table1[[#This Row],[10s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>-3.0392883617494482E-2</v>
+      </c>
+      <c r="N4" s="13">
         <v>447</v>
       </c>
+      <c r="O4" s="8">
+        <f t="shared" ref="O4:O19" si="5">(N4-N3)/N3</f>
+        <v>1.1699029126213591</v>
+      </c>
+      <c r="P4" s="9">
+        <f>(Table1[[#This Row],[1s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>-5.9303187546331038E-3</v>
+      </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:16">
       <c r="A5" s="1">
         <v>12</v>
       </c>
@@ -2328,43 +2459,59 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="12">
         <v>726.66666666666663</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="10">
         <f t="shared" si="1"/>
         <v>0.61601186063750912</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="12">
         <v>744.33333333333337</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="10">
         <f t="shared" si="2"/>
         <v>0.63950073421439069</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="8">
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>2.4311926605504693E-2</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="12">
         <v>988.66666666666663</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="10">
         <f t="shared" si="3"/>
         <v>0.66442199775533106</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="8">
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.36055045871559632</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="13">
         <v>717</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="8">
+        <f t="shared" si="4"/>
+        <v>0.64449541284403666</v>
+      </c>
+      <c r="M5" s="9">
+        <f>(Table1[[#This Row],[10s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>-1.330275229357793E-2</v>
+      </c>
+      <c r="N5" s="13">
         <v>785.5</v>
       </c>
+      <c r="O5" s="8">
+        <f t="shared" si="5"/>
+        <v>0.75727069351230425</v>
+      </c>
+      <c r="P5" s="9">
+        <f>(Table1[[#This Row],[1s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>8.0963302752293631E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:16">
       <c r="A6" s="1">
         <v>16</v>
       </c>
@@ -2372,43 +2519,59 @@
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="12">
         <v>1012.6666666666666</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="10">
         <f t="shared" si="1"/>
         <v>0.39357798165137614</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="12">
         <v>1043</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="10">
         <f t="shared" si="2"/>
         <v>0.40125391849529773</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="8">
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>2.9953917050691281E-2</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="12">
         <v>1337.6666666666667</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="10">
         <f t="shared" si="3"/>
         <v>0.35300067430883358</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="8">
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.32093482554312058</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="13">
         <v>1042</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="8">
+        <f t="shared" si="4"/>
+        <v>0.45327754532775455</v>
+      </c>
+      <c r="M6" s="9">
+        <f>(Table1[[#This Row],[10s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>2.8966425279789373E-2</v>
+      </c>
+      <c r="N6" s="13">
         <v>1076.5</v>
       </c>
+      <c r="O6" s="8">
+        <f t="shared" si="5"/>
+        <v>0.37046467218332274</v>
+      </c>
+      <c r="P6" s="9">
+        <f>(Table1[[#This Row],[1s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>6.3034891375905247E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:16">
       <c r="A7" s="1">
         <v>24</v>
       </c>
@@ -2416,43 +2579,59 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="12">
         <v>1586.3333333333333</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="10">
         <f t="shared" si="1"/>
         <v>0.56649111257406182</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="12">
         <v>1650.6666666666667</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="10">
         <f t="shared" si="2"/>
         <v>0.58261425375519338</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="8">
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>4.0554738390418253E-2</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="12">
         <v>2096.3333333333335</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="10">
         <f t="shared" si="3"/>
         <v>0.56715674059307253</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="8">
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.32149611262870365</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="13">
         <v>1640</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="8">
+        <f t="shared" si="4"/>
+        <v>0.57389635316698662</v>
+      </c>
+      <c r="M7" s="9">
+        <f>(Table1[[#This Row],[10s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>3.3830636688379961E-2</v>
+      </c>
+      <c r="N7" s="13">
         <v>1736</v>
       </c>
+      <c r="O7" s="8">
+        <f t="shared" si="5"/>
+        <v>0.61263353460287973</v>
+      </c>
+      <c r="P7" s="9">
+        <f>(Table1[[#This Row],[1s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>9.434755200672415E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:16">
       <c r="A8" s="1">
         <v>32</v>
       </c>
@@ -2460,43 +2639,59 @@
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="12">
         <v>2081.6666666666665</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="10">
         <f t="shared" si="1"/>
         <v>0.3122504727884009</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="12">
         <v>2314.3333333333335</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="10">
         <f t="shared" si="2"/>
         <v>0.40205977382875607</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="8">
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.1117694155324261</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="12">
         <v>2794.6666666666665</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="10">
         <f t="shared" si="3"/>
         <v>0.33312132294482411</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="8">
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.34251401120896718</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="13">
         <v>2221</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="8">
+        <f t="shared" si="4"/>
+        <v>0.35426829268292681</v>
+      </c>
+      <c r="M8" s="9">
+        <f>(Table1[[#This Row],[10s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>6.6933546837470048E-2</v>
+      </c>
+      <c r="N8" s="13">
         <v>2279</v>
       </c>
+      <c r="O8" s="8">
+        <f t="shared" si="5"/>
+        <v>0.31278801843317972</v>
+      </c>
+      <c r="P8" s="9">
+        <f>(Table1[[#This Row],[1s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>9.4795836669335554E-2</v>
+      </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:16">
       <c r="A9" s="1">
         <v>48</v>
       </c>
@@ -2504,43 +2699,59 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="12">
         <v>3241</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="10">
         <f t="shared" si="1"/>
         <v>0.55692554043234599</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="12">
         <v>3472.3333333333335</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="10">
         <f t="shared" si="2"/>
         <v>0.50036007489557821</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="8">
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>7.1377146971099495E-2</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="12">
         <v>4166.333333333333</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="10">
         <f t="shared" si="3"/>
         <v>0.49081583969465647</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="8">
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.2855085878843977</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="13">
         <v>3541</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="8">
+        <f t="shared" si="4"/>
+        <v>0.5943268797838811</v>
+      </c>
+      <c r="M9" s="9">
+        <f>(Table1[[#This Row],[10s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>9.2564023449552613E-2</v>
+      </c>
+      <c r="N9" s="13">
         <v>3522.5</v>
       </c>
+      <c r="O9" s="8">
+        <f t="shared" si="5"/>
+        <v>0.54563405002193943</v>
+      </c>
+      <c r="P9" s="9">
+        <f>(Table1[[#This Row],[1s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>8.6855908670163531E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:16">
       <c r="A10" s="1">
         <v>56</v>
       </c>
@@ -2548,43 +2759,59 @@
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="12">
         <v>3802</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="10">
         <f t="shared" si="1"/>
         <v>0.17309472385066338</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="12">
         <v>3942.6666666666665</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="10">
         <f t="shared" si="2"/>
         <v>0.1354516655467024</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="8">
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>3.6998071190601396E-2</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="12">
         <v>4331.333333333333</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="10">
         <f t="shared" si="3"/>
         <v>3.9603168253460282E-2</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="8">
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.13922496931439585</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="13">
         <v>3963</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="8">
+        <f t="shared" si="4"/>
+        <v>0.11917537418808247</v>
+      </c>
+      <c r="M10" s="9">
+        <f>(Table1[[#This Row],[10s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>4.2346133613887428E-2</v>
+      </c>
+      <c r="N10" s="13">
         <v>4018</v>
       </c>
+      <c r="O10" s="8">
+        <f t="shared" si="5"/>
+        <v>0.14066713981547196</v>
+      </c>
+      <c r="P10" s="9">
+        <f>(Table1[[#This Row],[1s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>5.6812204103103628E-2</v>
+      </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:16">
       <c r="A11" s="1">
         <v>64</v>
       </c>
@@ -2592,43 +2819,59 @@
         <f t="shared" si="0"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="12">
         <v>4068</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="10">
         <f t="shared" si="1"/>
         <v>6.996317727511836E-2</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="12">
         <v>4722</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="10">
         <f t="shared" si="2"/>
         <v>0.1976665539398039</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="8">
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.16076696165191739</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="12">
         <v>5431</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="10">
         <f t="shared" si="3"/>
         <v>0.25388640911189786</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="8">
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.33505408062930186</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="13">
         <v>4608</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="8">
+        <f t="shared" si="4"/>
+        <v>0.1627554882664648</v>
+      </c>
+      <c r="M11" s="9">
+        <f>(Table1[[#This Row],[10s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>0.13274336283185842</v>
+      </c>
+      <c r="N11" s="13">
         <v>4760</v>
       </c>
+      <c r="O11" s="8">
+        <f t="shared" si="5"/>
+        <v>0.18466898954703834</v>
+      </c>
+      <c r="P11" s="9">
+        <f>(Table1[[#This Row],[1s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>0.17010816125860373</v>
+      </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:16">
       <c r="A12" s="1">
         <v>96</v>
       </c>
@@ -2636,43 +2879,59 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="12">
         <v>6320.333333333333</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="10">
         <f t="shared" si="1"/>
         <v>0.5536709275647328</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="12">
         <v>6506</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="10">
         <f t="shared" si="2"/>
         <v>0.37780601440067768</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="8">
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>2.9376087759084485E-2</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="12">
         <v>8174</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="10">
         <f t="shared" si="3"/>
         <v>0.50506352421285217</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="8">
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.29328621908127217</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12" s="13">
         <v>7095</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="8">
+        <f t="shared" si="4"/>
+        <v>0.53971354166666663</v>
+      </c>
+      <c r="M12" s="9">
+        <f>(Table1[[#This Row],[10s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>0.12256737513844213</v>
+      </c>
+      <c r="N12" s="13">
         <v>6862.5</v>
       </c>
+      <c r="O12" s="8">
+        <f t="shared" si="5"/>
+        <v>0.44170168067226889</v>
+      </c>
+      <c r="P12" s="9">
+        <f>(Table1[[#This Row],[1s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>8.5781340646590418E-2</v>
+      </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:16">
       <c r="A13" s="1">
         <v>128</v>
       </c>
@@ -2680,43 +2939,59 @@
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="12">
         <v>8017.333333333333</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="10">
         <f t="shared" si="1"/>
         <v>0.26849849691471972</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="12">
         <v>9072.3333333333339</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="10">
         <f t="shared" si="2"/>
         <v>0.39445639922123177</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="8">
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.13158988857475482</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="12">
         <v>10364.333333333334</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="10">
         <f t="shared" si="3"/>
         <v>0.26796346138161659</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="8">
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.29274072842175297</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K13" s="13">
         <v>8944</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="8">
+        <f t="shared" si="4"/>
+        <v>0.26060606060606062</v>
+      </c>
+      <c r="M13" s="9">
+        <f>(Table1[[#This Row],[10s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>0.11558290370863133</v>
+      </c>
+      <c r="N13" s="13">
         <v>9599.5</v>
       </c>
+      <c r="O13" s="8">
+        <f t="shared" si="5"/>
+        <v>0.39883424408014573</v>
+      </c>
+      <c r="P13" s="9">
+        <f>(Table1[[#This Row],[1s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>0.19734325627806423</v>
+      </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:16">
       <c r="A14" s="1">
         <v>256</v>
       </c>
@@ -2724,43 +2999,59 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="12">
         <v>9777.3333333333339</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="10">
         <f t="shared" si="1"/>
         <v>0.21952436387826388</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="12">
         <v>10369.666666666666</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="10">
         <f t="shared" si="2"/>
         <v>0.14299886100598877</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="8">
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>6.0582299195417848E-2</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="12">
         <v>11890</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="10">
         <f t="shared" si="3"/>
         <v>0.14720355063840729</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="8">
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.21607800354561563</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K14" s="13">
         <v>11116</v>
       </c>
-      <c r="L14" s="5">
+      <c r="L14" s="8">
+        <f t="shared" si="4"/>
+        <v>0.2428443649373882</v>
+      </c>
+      <c r="M14" s="9">
+        <f>(Table1[[#This Row],[10s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>0.13691531433246959</v>
+      </c>
+      <c r="N14" s="13">
         <v>11370</v>
       </c>
+      <c r="O14" s="8">
+        <f t="shared" si="5"/>
+        <v>0.18443668941090682</v>
+      </c>
+      <c r="P14" s="9">
+        <f>(Table1[[#This Row],[1s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>0.16289376789854076</v>
+      </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:16">
       <c r="A15" s="1">
         <v>512</v>
       </c>
@@ -2768,43 +3059,59 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="12">
         <v>12696.666666666666</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="10">
         <f t="shared" si="1"/>
         <v>0.29858175371607787</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="12">
         <v>13770.333333333334</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="10">
         <f t="shared" si="2"/>
         <v>0.32794368189270001</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="8">
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>8.4562877395642E-2</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="12">
         <v>15466.333333333334</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="10">
         <f t="shared" si="3"/>
         <v>0.30078497336697507</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J15" s="8">
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.21814124442110802</v>
       </c>
-      <c r="K15" s="5">
+      <c r="K15" s="13">
         <v>13754</v>
       </c>
-      <c r="L15" s="5">
+      <c r="L15" s="8">
+        <f t="shared" si="4"/>
+        <v>0.23731558114429652</v>
+      </c>
+      <c r="M15" s="9">
+        <f>(Table1[[#This Row],[10s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>8.3276450511945446E-2</v>
+      </c>
+      <c r="N15" s="13">
         <v>14356.5</v>
       </c>
+      <c r="O15" s="8">
+        <f t="shared" si="5"/>
+        <v>0.26266490765171502</v>
+      </c>
+      <c r="P15" s="9">
+        <f>(Table1[[#This Row],[1s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>0.13072985035442378</v>
+      </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:16">
       <c r="A16" s="1">
         <v>1024</v>
       </c>
@@ -2812,43 +3119,59 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="12">
         <v>16797</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="10">
         <f t="shared" si="1"/>
         <v>0.32294565502756634</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="12">
         <v>17894.666666666668</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="10">
         <f t="shared" si="2"/>
         <v>0.29950860545617392</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="8">
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>6.5348971046417084E-2</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="12">
         <v>19193.666666666668</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="10">
         <f t="shared" si="3"/>
         <v>0.24099657320200871</v>
       </c>
-      <c r="J16" s="5">
+      <c r="J16" s="8">
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.14268420948185198</v>
       </c>
-      <c r="K16" s="5">
+      <c r="K16" s="13">
         <v>17954</v>
       </c>
-      <c r="L16" s="5">
+      <c r="L16" s="8">
+        <f t="shared" si="4"/>
+        <v>0.30536571179293298</v>
+      </c>
+      <c r="M16" s="9">
+        <f>(Table1[[#This Row],[10s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>6.8881347859736861E-2</v>
+      </c>
+      <c r="N16" s="13">
         <v>18526.5</v>
       </c>
+      <c r="O16" s="8">
+        <f t="shared" si="5"/>
+        <v>0.29046076690001044</v>
+      </c>
+      <c r="P16" s="9">
+        <f>(Table1[[#This Row],[1s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>0.1029648151455617</v>
+      </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:16">
       <c r="A17" s="1">
         <v>1280</v>
       </c>
@@ -2856,43 +3179,59 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="12">
         <v>17989</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="10">
         <f t="shared" si="1"/>
         <v>7.0965053283324406E-2</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="12">
         <v>19289.666666666668</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="10">
         <f t="shared" si="2"/>
         <v>7.795618806348259E-2</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="8">
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>7.2303444697685695E-2</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="12">
         <v>21436</v>
       </c>
-      <c r="I17" s="5">
+      <c r="I17" s="10">
         <f t="shared" si="3"/>
         <v>0.11682673103975262</v>
       </c>
-      <c r="J17" s="5">
+      <c r="J17" s="8">
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.19161709933848464</v>
       </c>
-      <c r="K17" s="5">
+      <c r="K17" s="13">
         <v>18906</v>
       </c>
-      <c r="L17" s="5">
+      <c r="L17" s="8">
+        <f t="shared" si="4"/>
+        <v>5.3024395677843381E-2</v>
+      </c>
+      <c r="M17" s="9">
+        <f>(Table1[[#This Row],[10s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>5.0975596197676359E-2</v>
+      </c>
+      <c r="N17" s="13">
         <v>19508</v>
       </c>
+      <c r="O17" s="8">
+        <f t="shared" si="5"/>
+        <v>5.2978166410277173E-2</v>
+      </c>
+      <c r="P17" s="9">
+        <f>(Table1[[#This Row],[1s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>8.4440491411418087E-2</v>
+      </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:16">
       <c r="A18" s="1">
         <v>1536</v>
       </c>
@@ -2900,43 +3239,59 @@
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="12">
         <v>19119</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="10">
         <f t="shared" si="1"/>
         <v>6.281616543443215E-2</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="12">
         <v>19812.333333333332</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="10">
         <f t="shared" si="2"/>
         <v>2.7095681625740772E-2</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="8">
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>3.6264100284184954E-2</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="12">
         <v>21494.666666666668</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I18" s="10">
         <f t="shared" si="3"/>
         <v>2.7368290103875668E-3</v>
       </c>
-      <c r="J18" s="5">
+      <c r="J18" s="8">
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.12425684746412824</v>
       </c>
-      <c r="K18" s="5">
+      <c r="K18" s="13">
         <v>19894</v>
       </c>
-      <c r="L18" s="5">
+      <c r="L18" s="8">
+        <f t="shared" si="4"/>
+        <v>5.2258542261715855E-2</v>
+      </c>
+      <c r="M18" s="9">
+        <f>(Table1[[#This Row],[10s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>4.0535592865735659E-2</v>
+      </c>
+      <c r="N18" s="13">
         <v>20535</v>
       </c>
+      <c r="O18" s="8">
+        <f t="shared" si="5"/>
+        <v>5.2645068689768301E-2</v>
+      </c>
+      <c r="P18" s="9">
+        <f>(Table1[[#This Row],[1s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>7.406245096500863E-2</v>
+      </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:16">
       <c r="A19" s="2">
         <v>2048</v>
       </c>
@@ -2944,40 +3299,56 @@
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="12">
         <v>20388</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="10">
         <f t="shared" si="1"/>
         <v>6.6373764318217482E-2</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="12">
         <v>21465.333333333332</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="10">
         <f t="shared" si="2"/>
         <v>8.3432878510019015E-2</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="8">
         <f>(Table1[[#This Row],[5m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>5.2841540775619589E-2</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="12">
         <v>22838.333333333332</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I19" s="10">
         <f t="shared" si="3"/>
         <v>6.2511630792134371E-2</v>
       </c>
-      <c r="J19" s="5">
+      <c r="J19" s="8">
         <f>(Table1[[#This Row],[1m]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
         <v>0.12018507618860762</v>
       </c>
-      <c r="K19" s="5">
+      <c r="K19" s="13">
         <v>21284</v>
       </c>
-      <c r="L19" s="5">
+      <c r="L19" s="8">
+        <f t="shared" si="4"/>
+        <v>6.9870312657082531E-2</v>
+      </c>
+      <c r="M19" s="9">
+        <f>(Table1[[#This Row],[10s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>4.3947420051010398E-2</v>
+      </c>
+      <c r="N19" s="13">
         <v>22152</v>
+      </c>
+      <c r="O19" s="8">
+        <f t="shared" si="5"/>
+        <v>7.8743608473338209E-2</v>
+      </c>
+      <c r="P19" s="9">
+        <f>(Table1[[#This Row],[1s]]-Table1[[#This Row],[baseline]])/Table1[[#This Row],[baseline]]</f>
+        <v>8.6521483225426715E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>